<commit_message>
Criou alguns scripts R
</commit_message>
<xml_diff>
--- a/eda/mapa_coropleto/tic_domicilios_2024_g2a_3.xlsx
+++ b/eda/mapa_coropleto/tic_domicilios_2024_g2a_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Master-Dissertation\eda\tic_domicilios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Master-Dissertation\eda\mapa_coropleto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C641A4B6-ECDF-46CB-8315-88ECE7BB42D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA79064-2D62-4A3F-B051-3C03B565B142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Região</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
   </si>
 </sst>
 </file>
@@ -237,7 +231,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C6638A-B919-46BA-B9C9-5FD41D8A7D1C}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E2" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -539,14 +533,8 @@
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -559,14 +547,8 @@
       <c r="D2" s="5">
         <v>13</v>
       </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -579,14 +561,8 @@
       <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -599,14 +575,8 @@
       <c r="D4" s="4">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -619,14 +589,8 @@
       <c r="D5" s="3">
         <v>13</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -638,12 +602,6 @@
       </c>
       <c r="D6" s="6">
         <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>